<commit_message>
Added to analytics: regression models, handling for 2-part (delayed) treatment+test
</commit_message>
<xml_diff>
--- a/html/v2akureytemplate/ContentGuide.xlsx
+++ b/html/v2akureytemplate/ContentGuide.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\src\ssascams\html\v2akureytemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83043637-94C0-45D3-9F53-518BC664AB35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0A1B44-1182-46DF-A535-FCDACF9D9A3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="630" windowWidth="18330" windowHeight="10140" xr2:uid="{FFF5FB0D-EE95-4AAB-B906-4CB4BCED37BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FFF5FB0D-EE95-4AAB-B906-4CB4BCED37BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Content!$A$1:$K$19</definedName>
-    <definedName name="_Hlk71352808" localSheetId="0">Content!$C$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Content!$B$1:$L$19</definedName>
+    <definedName name="_Hlk71352808" localSheetId="0">Content!$D$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
   <si>
     <t>Stage</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>ssaInfo-1</t>
+  </si>
+  <si>
+    <t>Checked In Rainloop</t>
   </si>
 </sst>
 </file>
@@ -705,512 +708,527 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC92886-E0D2-4BE1-AA33-429C2443FEF3}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="40" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>64</v>
-      </c>
-      <c r="G2" t="s">
-        <v>37</v>
       </c>
       <c r="H2" t="s">
         <v>37</v>
       </c>
       <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>64</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
       </c>
       <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
         <v>11</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>47</v>
       </c>
       <c r="H7" t="s">
         <v>47</v>
       </c>
       <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>63</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>64</v>
-      </c>
-      <c r="G8" t="s">
-        <v>37</v>
       </c>
       <c r="H8" t="s">
         <v>37</v>
       </c>
       <c r="I8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>99</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>53</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>50</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
       </c>
       <c r="H9" t="s">
         <v>54</v>
       </c>
       <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" t="s">
         <v>13</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>95</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>50</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>51</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>52</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>13</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>96</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>59</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>60</v>
-      </c>
-      <c r="G11" t="s">
-        <v>61</v>
       </c>
       <c r="H11" t="s">
         <v>61</v>
       </c>
       <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s">
         <v>13</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>93</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>55</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>56</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>57</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>58</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>13</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>94</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>65</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>66</v>
-      </c>
-      <c r="G13" t="s">
-        <v>67</v>
       </c>
       <c r="H13" t="s">
         <v>67</v>
       </c>
       <c r="I13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" t="s">
         <v>13</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>98</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>85</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>64</v>
-      </c>
-      <c r="G14" t="s">
-        <v>37</v>
       </c>
       <c r="H14" t="s">
         <v>37</v>
       </c>
       <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" t="s">
         <v>13</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>97</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>36</v>
-      </c>
-      <c r="F15" t="s">
-        <v>62</v>
       </c>
       <c r="G15" t="s">
         <v>62</v>
@@ -1219,145 +1237,148 @@
         <v>62</v>
       </c>
       <c r="I15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" t="s">
         <v>13</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>92</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>83</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>84</v>
-      </c>
-      <c r="G16" t="s">
-        <v>47</v>
       </c>
       <c r="H16" t="s">
         <v>47</v>
       </c>
       <c r="I16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" t="s">
         <v>11</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>87</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>88</v>
-      </c>
-      <c r="G17" t="s">
-        <v>47</v>
       </c>
       <c r="H17" t="s">
         <v>47</v>
       </c>
       <c r="I17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" t="s">
         <v>11</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>81</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>82</v>
-      </c>
-      <c r="G18" t="s">
-        <v>47</v>
       </c>
       <c r="H18" t="s">
         <v>47</v>
       </c>
       <c r="I18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" t="s">
         <v>11</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>16</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="G19" t="s">
-        <v>47</v>
       </c>
       <c r="H19" t="s">
         <v>47</v>
       </c>
       <c r="I19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" t="s">
         <v>11</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K19" xr:uid="{3878B2FF-54B4-4707-BF0B-BF38ED6B1364}">
+  <autoFilter ref="B1:L19" xr:uid="{3878B2FF-54B4-4707-BF0B-BF38ED6B1364}">
     <filterColumn colId="8">
       <filters>
         <filter val="Yes"/>

</xml_diff>